<commit_message>
update feature analysis results
</commit_message>
<xml_diff>
--- a/output/validator/simulated-results.xlsx
+++ b/output/validator/simulated-results.xlsx
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -618,7 +618,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -668,7 +668,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -818,7 +818,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -868,7 +868,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -918,7 +918,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1018,7 +1018,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1068,7 +1068,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1718,7 +1718,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -2118,7 +2118,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -2318,7 +2318,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -2418,7 +2418,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -2468,7 +2468,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -2518,7 +2518,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -2618,7 +2618,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -2668,7 +2668,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -2718,7 +2718,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -2818,7 +2818,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -2868,7 +2868,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2918,7 +2918,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -3018,7 +3018,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -3068,7 +3068,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -3118,7 +3118,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -3168,7 +3168,7 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -3218,7 +3218,7 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -3268,7 +3268,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -3318,7 +3318,7 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -3418,7 +3418,7 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -3468,7 +3468,7 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -3518,7 +3518,7 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -3568,7 +3568,7 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
@@ -3618,7 +3618,7 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -3668,7 +3668,7 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
@@ -3918,7 +3918,7 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
@@ -4018,7 +4018,7 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
@@ -4068,7 +4068,7 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
@@ -4118,7 +4118,7 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
@@ -4168,7 +4168,7 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
@@ -4218,7 +4218,7 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
@@ -4268,7 +4268,7 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
@@ -4318,7 +4318,7 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
@@ -4368,7 +4368,7 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
@@ -4418,7 +4418,7 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
@@ -4468,7 +4468,7 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
@@ -4518,7 +4518,7 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
@@ -4568,7 +4568,7 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
@@ -4618,7 +4618,7 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
@@ -4668,7 +4668,7 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
@@ -5318,7 +5318,7 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
@@ -5368,7 +5368,7 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
@@ -5918,7 +5918,7 @@
         </is>
       </c>
       <c r="E110" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F110" t="inlineStr">
         <is>
@@ -5968,7 +5968,7 @@
         </is>
       </c>
       <c r="E111" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F111" t="inlineStr">
         <is>
@@ -6018,7 +6018,7 @@
         </is>
       </c>
       <c r="E112" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F112" t="inlineStr">
         <is>
@@ -6068,7 +6068,7 @@
         </is>
       </c>
       <c r="E113" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F113" t="inlineStr">
         <is>
@@ -6118,7 +6118,7 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F114" t="inlineStr">
         <is>
@@ -6168,7 +6168,7 @@
         </is>
       </c>
       <c r="E115" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F115" t="inlineStr">
         <is>
@@ -6218,7 +6218,7 @@
         </is>
       </c>
       <c r="E116" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F116" t="inlineStr">
         <is>
@@ -6268,7 +6268,7 @@
         </is>
       </c>
       <c r="E117" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F117" t="inlineStr">
         <is>
@@ -6318,7 +6318,7 @@
         </is>
       </c>
       <c r="E118" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F118" t="inlineStr">
         <is>
@@ -6368,7 +6368,7 @@
         </is>
       </c>
       <c r="E119" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F119" t="inlineStr">
         <is>
@@ -6418,7 +6418,7 @@
         </is>
       </c>
       <c r="E120" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F120" t="inlineStr">
         <is>
@@ -6468,7 +6468,7 @@
         </is>
       </c>
       <c r="E121" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F121" t="inlineStr">
         <is>
@@ -6518,7 +6518,7 @@
         </is>
       </c>
       <c r="E122" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F122" t="inlineStr">
         <is>
@@ -6568,7 +6568,7 @@
         </is>
       </c>
       <c r="E123" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F123" t="inlineStr">
         <is>
@@ -6618,7 +6618,7 @@
         </is>
       </c>
       <c r="E124" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F124" t="inlineStr">
         <is>
@@ -6668,7 +6668,7 @@
         </is>
       </c>
       <c r="E125" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
@@ -6718,7 +6718,7 @@
         </is>
       </c>
       <c r="E126" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
@@ -6768,7 +6768,7 @@
         </is>
       </c>
       <c r="E127" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F127" t="inlineStr">
         <is>
@@ -6818,7 +6818,7 @@
         </is>
       </c>
       <c r="E128" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F128" t="inlineStr">
         <is>
@@ -6868,7 +6868,7 @@
         </is>
       </c>
       <c r="E129" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F129" t="inlineStr">
         <is>
@@ -6918,7 +6918,7 @@
         </is>
       </c>
       <c r="E130" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F130" t="inlineStr">
         <is>
@@ -6968,7 +6968,7 @@
         </is>
       </c>
       <c r="E131" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F131" t="inlineStr">
         <is>
@@ -7018,7 +7018,7 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F132" t="inlineStr">
         <is>
@@ -7068,7 +7068,7 @@
         </is>
       </c>
       <c r="E133" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F133" t="inlineStr">
         <is>
@@ -7118,7 +7118,7 @@
         </is>
       </c>
       <c r="E134" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F134" t="inlineStr">
         <is>
@@ -7168,7 +7168,7 @@
         </is>
       </c>
       <c r="E135" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F135" t="inlineStr">
         <is>
@@ -7218,7 +7218,7 @@
         </is>
       </c>
       <c r="E136" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F136" t="inlineStr">
         <is>
@@ -7268,7 +7268,7 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
@@ -7318,7 +7318,7 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F138" t="inlineStr">
         <is>
@@ -7368,7 +7368,7 @@
         </is>
       </c>
       <c r="E139" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F139" t="inlineStr">
         <is>
@@ -7418,7 +7418,7 @@
         </is>
       </c>
       <c r="E140" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F140" t="inlineStr">
         <is>
@@ -7468,7 +7468,7 @@
         </is>
       </c>
       <c r="E141" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F141" t="inlineStr">
         <is>
@@ -7518,7 +7518,7 @@
         </is>
       </c>
       <c r="E142" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F142" t="inlineStr">
         <is>
@@ -7568,7 +7568,7 @@
         </is>
       </c>
       <c r="E143" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F143" t="inlineStr">
         <is>
@@ -7618,7 +7618,7 @@
         </is>
       </c>
       <c r="E144" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F144" t="inlineStr">
         <is>
@@ -7668,7 +7668,7 @@
         </is>
       </c>
       <c r="E145" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F145" t="inlineStr">
         <is>
@@ -7718,7 +7718,7 @@
         </is>
       </c>
       <c r="E146" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F146" t="inlineStr">
         <is>
@@ -7768,7 +7768,7 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F147" t="inlineStr">
         <is>
@@ -7818,7 +7818,7 @@
         </is>
       </c>
       <c r="E148" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F148" t="inlineStr">
         <is>
@@ -7868,7 +7868,7 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F149" t="inlineStr">
         <is>
@@ -7918,7 +7918,7 @@
         </is>
       </c>
       <c r="E150" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F150" t="inlineStr">
         <is>
@@ -7968,7 +7968,7 @@
         </is>
       </c>
       <c r="E151" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F151" t="inlineStr">
         <is>
@@ -8018,7 +8018,7 @@
         </is>
       </c>
       <c r="E152" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F152" t="inlineStr">
         <is>
@@ -8068,7 +8068,7 @@
         </is>
       </c>
       <c r="E153" t="n">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="F153" t="inlineStr">
         <is>
@@ -8118,7 +8118,7 @@
         </is>
       </c>
       <c r="E154" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F154" t="inlineStr">
         <is>
@@ -8168,7 +8168,7 @@
         </is>
       </c>
       <c r="E155" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F155" t="inlineStr">
         <is>
@@ -8218,7 +8218,7 @@
         </is>
       </c>
       <c r="E156" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F156" t="inlineStr">
         <is>
@@ -8268,7 +8268,7 @@
         </is>
       </c>
       <c r="E157" t="n">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="F157" t="inlineStr">
         <is>
@@ -8368,7 +8368,7 @@
         </is>
       </c>
       <c r="E159" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="F159" t="inlineStr">
         <is>
@@ -8568,7 +8568,7 @@
         </is>
       </c>
       <c r="E163" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F163" t="inlineStr">
         <is>
@@ -8718,7 +8718,7 @@
         </is>
       </c>
       <c r="E166" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F166" t="inlineStr">
         <is>
@@ -8768,7 +8768,7 @@
         </is>
       </c>
       <c r="E167" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F167" t="inlineStr">
         <is>
@@ -8918,7 +8918,7 @@
         </is>
       </c>
       <c r="E170" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F170" t="inlineStr">
         <is>
@@ -9168,7 +9168,7 @@
         </is>
       </c>
       <c r="E175" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F175" t="inlineStr">
         <is>
@@ -9568,7 +9568,7 @@
         </is>
       </c>
       <c r="E183" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F183" t="inlineStr">
         <is>
@@ -9618,7 +9618,7 @@
         </is>
       </c>
       <c r="E184" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F184" t="inlineStr">
         <is>
@@ -9668,7 +9668,7 @@
         </is>
       </c>
       <c r="E185" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F185" t="inlineStr">
         <is>
@@ -9718,7 +9718,7 @@
         </is>
       </c>
       <c r="E186" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F186" t="inlineStr">
         <is>
@@ -9768,7 +9768,7 @@
         </is>
       </c>
       <c r="E187" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F187" t="inlineStr">
         <is>
@@ -9818,7 +9818,7 @@
         </is>
       </c>
       <c r="E188" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F188" t="inlineStr">
         <is>
@@ -9868,7 +9868,7 @@
         </is>
       </c>
       <c r="E189" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F189" t="inlineStr">
         <is>
@@ -10168,7 +10168,7 @@
         </is>
       </c>
       <c r="E195" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F195" t="inlineStr">
         <is>
@@ -10218,7 +10218,7 @@
         </is>
       </c>
       <c r="E196" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F196" t="inlineStr">
         <is>
@@ -10268,7 +10268,7 @@
         </is>
       </c>
       <c r="E197" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F197" t="inlineStr">
         <is>
@@ -10318,7 +10318,7 @@
         </is>
       </c>
       <c r="E198" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F198" t="inlineStr">
         <is>
@@ -10368,7 +10368,7 @@
         </is>
       </c>
       <c r="E199" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F199" t="inlineStr">
         <is>
@@ -10418,7 +10418,7 @@
         </is>
       </c>
       <c r="E200" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F200" t="inlineStr">
         <is>
@@ -10468,7 +10468,7 @@
         </is>
       </c>
       <c r="E201" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F201" t="inlineStr">
         <is>
@@ -10518,7 +10518,7 @@
         </is>
       </c>
       <c r="E202" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F202" t="inlineStr">
         <is>
@@ -10568,7 +10568,7 @@
         </is>
       </c>
       <c r="E203" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F203" t="inlineStr">
         <is>
@@ -10618,7 +10618,7 @@
         </is>
       </c>
       <c r="E204" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F204" t="inlineStr">
         <is>
@@ -10668,7 +10668,7 @@
         </is>
       </c>
       <c r="E205" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="F205" t="inlineStr">
         <is>
@@ -10718,7 +10718,7 @@
         </is>
       </c>
       <c r="E206" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F206" t="inlineStr">
         <is>
@@ -10768,7 +10768,7 @@
         </is>
       </c>
       <c r="E207" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F207" t="inlineStr">
         <is>
@@ -10818,7 +10818,7 @@
         </is>
       </c>
       <c r="E208" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F208" t="inlineStr">
         <is>
@@ -10868,7 +10868,7 @@
         </is>
       </c>
       <c r="E209" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F209" t="inlineStr">
         <is>
@@ -10968,7 +10968,7 @@
         </is>
       </c>
       <c r="E211" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F211" t="inlineStr">
         <is>
@@ -11018,7 +11018,7 @@
         </is>
       </c>
       <c r="E212" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F212" t="inlineStr">
         <is>
@@ -11068,7 +11068,7 @@
         </is>
       </c>
       <c r="E213" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F213" t="inlineStr">
         <is>
@@ -11168,7 +11168,7 @@
         </is>
       </c>
       <c r="E215" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F215" t="inlineStr">
         <is>
@@ -11218,7 +11218,7 @@
         </is>
       </c>
       <c r="E216" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F216" t="inlineStr">
         <is>
@@ -11268,7 +11268,7 @@
         </is>
       </c>
       <c r="E217" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="F217" t="inlineStr">
         <is>

</xml_diff>